<commit_message>
permirsim i regjistrit bodrum
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
@@ -362,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,18 +510,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -1011,7 +999,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1104,6 +1092,168 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1158,15 +1308,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1175,189 +1316,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1736,8 +1694,8 @@
   </sheetPr>
   <dimension ref="B1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,244 +1718,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="34"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="91"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="37"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="91"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="37"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="91"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="37"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="91"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="37"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="91"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="37"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="91"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="37"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="91"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="91"/>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="40"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="93"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="94"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="43"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="97"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="99"/>
+      <c r="N12" s="99"/>
+      <c r="O12" s="99"/>
+      <c r="P12" s="99"/>
+      <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="49"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
+      <c r="O13" s="102"/>
+      <c r="P13" s="102"/>
+      <c r="Q13" s="103"/>
     </row>
     <row r="14" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -2012,18 +1970,18 @@
       <c r="E14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="56" t="s">
+      <c r="F14" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56" t="s">
+      <c r="G14" s="63"/>
+      <c r="H14" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="56"/>
-      <c r="J14" s="74" t="s">
+      <c r="I14" s="63"/>
+      <c r="J14" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="75"/>
+      <c r="K14" s="70"/>
       <c r="L14" s="8" t="s">
         <v>17</v>
       </c>
@@ -2056,18 +2014,18 @@
       <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="64">
         <v>411.35</v>
       </c>
-      <c r="G15" s="69"/>
-      <c r="H15" s="70" t="s">
+      <c r="G15" s="64"/>
+      <c r="H15" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="76" t="s">
+      <c r="I15" s="65"/>
+      <c r="J15" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="77"/>
+      <c r="K15" s="72"/>
       <c r="L15" s="11" t="s">
         <v>33</v>
       </c>
@@ -2088,62 +2046,62 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72"/>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="73"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="68"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="55"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="105"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="105"/>
+      <c r="Q17" s="106"/>
     </row>
     <row r="18" spans="2:17" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="28" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="61"/>
+      <c r="I18" s="77"/>
       <c r="J18" s="28" t="s">
         <v>6</v>
       </c>
@@ -2173,21 +2131,21 @@
       <c r="B19" s="22">
         <v>1</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="82"/>
       <c r="F19" s="23">
         <v>3</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="62">
-        <v>17.91</v>
-      </c>
-      <c r="I19" s="63"/>
+      <c r="H19" s="58">
+        <v>18.02</v>
+      </c>
+      <c r="I19" s="59"/>
       <c r="J19" s="23" t="s">
         <v>34</v>
       </c>
@@ -2217,21 +2175,21 @@
       <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
       <c r="F20" s="23">
         <v>3</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="62">
-        <v>14.75</v>
-      </c>
-      <c r="I20" s="63"/>
+      <c r="H20" s="58">
+        <v>14.64</v>
+      </c>
+      <c r="I20" s="59"/>
       <c r="J20" s="23" t="s">
         <v>34</v>
       </c>
@@ -2258,46 +2216,46 @@
       </c>
     </row>
     <row r="21" spans="2:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="78">
+      <c r="B21" s="4">
         <v>3</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="82">
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="23">
         <v>4</v>
       </c>
-      <c r="G21" s="83" t="s">
+      <c r="G21" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="84">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="I21" s="85"/>
-      <c r="J21" s="82" t="s">
+      <c r="H21" s="58">
+        <v>14.36</v>
+      </c>
+      <c r="I21" s="59"/>
+      <c r="J21" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K21" s="82" t="s">
+      <c r="K21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="82" t="s">
+      <c r="L21" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="M21" s="83" t="s">
+      <c r="M21" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="N21" s="82" t="s">
+      <c r="N21" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="82">
+      <c r="O21" s="23">
         <v>1005022530</v>
       </c>
-      <c r="P21" s="86" t="s">
+      <c r="P21" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="Q21" s="87" t="s">
+      <c r="Q21" s="26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2305,21 +2263,21 @@
       <c r="B22" s="4">
         <v>4</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="82"/>
       <c r="F22" s="23">
         <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="62">
-        <v>253.56</v>
-      </c>
-      <c r="I22" s="63"/>
+      <c r="H22" s="58">
+        <v>254.43</v>
+      </c>
+      <c r="I22" s="59"/>
       <c r="J22" s="23" t="s">
         <v>34</v>
       </c>
@@ -2349,21 +2307,21 @@
       <c r="B23" s="22">
         <v>5</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="23">
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="62">
+      <c r="H23" s="58">
         <v>333.84</v>
       </c>
-      <c r="I23" s="63"/>
+      <c r="I23" s="59"/>
       <c r="J23" s="23" t="s">
         <v>34</v>
       </c>
@@ -2393,21 +2351,21 @@
       <c r="B24" s="4">
         <v>6</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
       <c r="F24" s="23">
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="62">
+      <c r="H24" s="58">
         <v>11.53</v>
       </c>
-      <c r="I24" s="63"/>
+      <c r="I24" s="59"/>
       <c r="J24" s="23" t="s">
         <v>34</v>
       </c>
@@ -2437,21 +2395,21 @@
       <c r="B25" s="22">
         <v>7</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="23">
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="62">
+      <c r="H25" s="58">
         <v>12.41</v>
       </c>
-      <c r="I25" s="63"/>
+      <c r="I25" s="59"/>
       <c r="J25" s="23" t="s">
         <v>34</v>
       </c>
@@ -2481,21 +2439,21 @@
       <c r="B26" s="4">
         <v>8</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="89"/>
-      <c r="E26" s="90"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="58">
         <v>333.67</v>
       </c>
-      <c r="I26" s="63"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="23" t="s">
         <v>34</v>
       </c>
@@ -2525,21 +2483,21 @@
       <c r="B27" s="4">
         <v>9</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="90"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="1">
         <v>2</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
       </c>
-      <c r="H27" s="62">
+      <c r="H27" s="58">
         <v>12.28</v>
       </c>
-      <c r="I27" s="63"/>
+      <c r="I27" s="59"/>
       <c r="J27" s="23" t="s">
         <v>34</v>
       </c>
@@ -2569,21 +2527,21 @@
       <c r="B28" s="4">
         <v>10</v>
       </c>
-      <c r="C28" s="88" t="s">
+      <c r="C28" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="90"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="H28" s="62">
+      <c r="H28" s="58">
         <v>11.82</v>
       </c>
-      <c r="I28" s="63"/>
+      <c r="I28" s="59"/>
       <c r="J28" s="23" t="s">
         <v>34</v>
       </c>
@@ -2610,24 +2568,24 @@
       </c>
     </row>
     <row r="29" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="94">
+      <c r="B29" s="35">
         <v>11</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="89"/>
-      <c r="E29" s="90"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
       </c>
-      <c r="H29" s="62">
+      <c r="H29" s="58">
         <v>22.2</v>
       </c>
-      <c r="I29" s="63"/>
+      <c r="I29" s="59"/>
       <c r="J29" s="23" t="s">
         <v>34</v>
       </c>
@@ -2654,24 +2612,24 @@
       </c>
     </row>
     <row r="30" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="94">
+      <c r="B30" s="35">
         <v>12</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="89"/>
-      <c r="E30" s="90"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="62"/>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="2">
         <v>2</v>
       </c>
-      <c r="H30" s="62">
+      <c r="H30" s="58">
         <v>20.6</v>
       </c>
-      <c r="I30" s="63"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="23" t="s">
         <v>34</v>
       </c>
@@ -2698,24 +2656,24 @@
       </c>
     </row>
     <row r="31" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="94">
+      <c r="B31" s="35">
         <v>13</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C31" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="89"/>
-      <c r="E31" s="90"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="62"/>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="2">
         <v>2</v>
       </c>
-      <c r="H31" s="62">
+      <c r="H31" s="58">
         <v>31.12</v>
       </c>
-      <c r="I31" s="63"/>
+      <c r="I31" s="59"/>
       <c r="J31" s="23" t="s">
         <v>34</v>
       </c>
@@ -2742,24 +2700,24 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="94">
+      <c r="B32" s="35">
         <v>14</v>
       </c>
-      <c r="C32" s="88" t="s">
+      <c r="C32" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="90"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="62"/>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="2">
         <v>2</v>
       </c>
-      <c r="H32" s="62">
+      <c r="H32" s="58">
         <v>32.97</v>
       </c>
-      <c r="I32" s="63"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="23" t="s">
         <v>34</v>
       </c>
@@ -2786,24 +2744,24 @@
       </c>
     </row>
     <row r="33" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="94">
+      <c r="B33" s="35">
         <v>15</v>
       </c>
-      <c r="C33" s="88" t="s">
+      <c r="C33" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="89"/>
-      <c r="E33" s="90"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="62"/>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="2">
         <v>2</v>
       </c>
-      <c r="H33" s="62">
+      <c r="H33" s="58">
         <v>30.53</v>
       </c>
-      <c r="I33" s="63">
+      <c r="I33" s="59">
         <v>30.53</v>
       </c>
       <c r="J33" s="23" t="s">
@@ -2832,24 +2790,24 @@
       </c>
     </row>
     <row r="34" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="94">
+      <c r="B34" s="35">
         <v>16</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C34" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="89"/>
-      <c r="E34" s="90"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="2">
         <v>2</v>
       </c>
-      <c r="H34" s="62">
+      <c r="H34" s="58">
         <v>26.02</v>
       </c>
-      <c r="I34" s="63">
+      <c r="I34" s="59">
         <v>26.02</v>
       </c>
       <c r="J34" s="23" t="s">
@@ -2878,24 +2836,24 @@
       </c>
     </row>
     <row r="35" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="94">
+      <c r="B35" s="35">
         <v>17</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="90"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="62"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="2">
         <v>2</v>
       </c>
-      <c r="H35" s="62">
+      <c r="H35" s="58">
         <v>4.92</v>
       </c>
-      <c r="I35" s="63">
+      <c r="I35" s="59">
         <v>4.92</v>
       </c>
       <c r="J35" s="23" t="s">
@@ -2924,24 +2882,24 @@
       </c>
     </row>
     <row r="36" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B36" s="94">
+      <c r="B36" s="35">
         <v>18</v>
       </c>
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="89"/>
-      <c r="E36" s="90"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="62"/>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="2">
         <v>2</v>
       </c>
-      <c r="H36" s="62">
+      <c r="H36" s="58">
         <v>36.840000000000003</v>
       </c>
-      <c r="I36" s="63">
+      <c r="I36" s="59">
         <v>36.840000000000003</v>
       </c>
       <c r="J36" s="23" t="s">
@@ -2970,24 +2928,24 @@
       </c>
     </row>
     <row r="37" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="94">
+      <c r="B37" s="35">
         <v>19</v>
       </c>
-      <c r="C37" s="88" t="s">
+      <c r="C37" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="89"/>
-      <c r="E37" s="90"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="62"/>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="2">
         <v>2</v>
       </c>
-      <c r="H37" s="62">
+      <c r="H37" s="58">
         <v>37.39</v>
       </c>
-      <c r="I37" s="63">
+      <c r="I37" s="59">
         <v>37.39</v>
       </c>
       <c r="J37" s="23" t="s">
@@ -3016,24 +2974,24 @@
       </c>
     </row>
     <row r="38" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="94">
+      <c r="B38" s="35">
         <v>20</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="89"/>
-      <c r="E38" s="90"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="H38" s="62">
+      <c r="H38" s="58">
         <v>35.07</v>
       </c>
-      <c r="I38" s="63">
+      <c r="I38" s="59">
         <v>35.07</v>
       </c>
       <c r="J38" s="23" t="s">
@@ -3062,24 +3020,24 @@
       </c>
     </row>
     <row r="39" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="94">
+      <c r="B39" s="35">
         <v>21</v>
       </c>
-      <c r="C39" s="88" t="s">
+      <c r="C39" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="89"/>
-      <c r="E39" s="90"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="62"/>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="2">
         <v>2</v>
       </c>
-      <c r="H39" s="62">
+      <c r="H39" s="58">
         <v>37.89</v>
       </c>
-      <c r="I39" s="63">
+      <c r="I39" s="59">
         <v>37.89</v>
       </c>
       <c r="J39" s="23" t="s">
@@ -3108,14 +3066,14 @@
       </c>
     </row>
     <row r="40" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="94">
+      <c r="B40" s="35">
         <v>22</v>
       </c>
-      <c r="C40" s="88" t="s">
+      <c r="C40" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="89"/>
-      <c r="E40" s="90"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="62"/>
       <c r="F40" s="1">
         <v>1</v>
       </c>
@@ -3152,24 +3110,24 @@
       </c>
     </row>
     <row r="41" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="94">
+      <c r="B41" s="35">
         <v>23</v>
       </c>
-      <c r="C41" s="88" t="s">
+      <c r="C41" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="89"/>
-      <c r="E41" s="90"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="62"/>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="2">
         <v>3</v>
       </c>
-      <c r="H41" s="62">
+      <c r="H41" s="58">
         <v>73.92</v>
       </c>
-      <c r="I41" s="63">
+      <c r="I41" s="59">
         <v>17.11</v>
       </c>
       <c r="J41" s="23" t="s">
@@ -3198,24 +3156,24 @@
       </c>
     </row>
     <row r="42" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="94">
+      <c r="B42" s="35">
         <v>24</v>
       </c>
-      <c r="C42" s="88" t="s">
+      <c r="C42" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="89"/>
-      <c r="E42" s="90"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="62"/>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="2">
         <v>3</v>
       </c>
-      <c r="H42" s="62">
+      <c r="H42" s="58">
         <v>32.96</v>
       </c>
-      <c r="I42" s="63"/>
+      <c r="I42" s="59"/>
       <c r="J42" s="23" t="s">
         <v>34</v>
       </c>
@@ -3242,24 +3200,24 @@
       </c>
     </row>
     <row r="43" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="94">
+      <c r="B43" s="35">
         <v>25</v>
       </c>
-      <c r="C43" s="88" t="s">
+      <c r="C43" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="89"/>
-      <c r="E43" s="90"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62"/>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="2">
         <v>3</v>
       </c>
-      <c r="H43" s="62">
+      <c r="H43" s="58">
         <v>76.430000000000007</v>
       </c>
-      <c r="I43" s="63"/>
+      <c r="I43" s="59"/>
       <c r="J43" s="23" t="s">
         <v>34</v>
       </c>
@@ -3286,24 +3244,24 @@
       </c>
     </row>
     <row r="44" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="94">
+      <c r="B44" s="35">
         <v>26</v>
       </c>
-      <c r="C44" s="88" t="s">
+      <c r="C44" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="89"/>
-      <c r="E44" s="90"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="2">
         <v>3</v>
       </c>
-      <c r="H44" s="62">
+      <c r="H44" s="58">
         <v>86.27</v>
       </c>
-      <c r="I44" s="63"/>
+      <c r="I44" s="59"/>
       <c r="J44" s="23" t="s">
         <v>34</v>
       </c>
@@ -3330,24 +3288,24 @@
       </c>
     </row>
     <row r="45" spans="2:17" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="94">
+      <c r="B45" s="35">
         <v>27</v>
       </c>
-      <c r="C45" s="88" t="s">
+      <c r="C45" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="89"/>
-      <c r="E45" s="90"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="62"/>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="2">
         <v>3</v>
       </c>
-      <c r="H45" s="62">
+      <c r="H45" s="58">
         <v>85.22</v>
       </c>
-      <c r="I45" s="63"/>
+      <c r="I45" s="59"/>
       <c r="J45" s="23" t="s">
         <v>34</v>
       </c>
@@ -3375,9 +3333,9 @@
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="92"/>
-      <c r="E46" s="93"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="34"/>
       <c r="F46" s="1"/>
       <c r="G46" s="2"/>
       <c r="H46" s="30"/>
@@ -3393,9 +3351,9 @@
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="91"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="93"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="34"/>
       <c r="F47" s="1"/>
       <c r="G47" s="2"/>
       <c r="H47" s="30"/>
@@ -3411,9 +3369,9 @@
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="93"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="34"/>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
       <c r="H48" s="30"/>
@@ -3429,9 +3387,9 @@
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="91"/>
-      <c r="D49" s="92"/>
-      <c r="E49" s="93"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="34"/>
       <c r="F49" s="1"/>
       <c r="G49" s="2"/>
       <c r="H49" s="30"/>
@@ -3447,9 +3405,9 @@
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
-      <c r="C50" s="91"/>
-      <c r="D50" s="92"/>
-      <c r="E50" s="93"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="34"/>
       <c r="F50" s="1"/>
       <c r="G50" s="2"/>
       <c r="H50" s="30"/>
@@ -3465,9 +3423,9 @@
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="93"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="34"/>
       <c r="F51" s="1"/>
       <c r="G51" s="2"/>
       <c r="H51" s="30"/>
@@ -3483,9 +3441,9 @@
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
-      <c r="C52" s="91"/>
-      <c r="D52" s="92"/>
-      <c r="E52" s="93"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="34"/>
       <c r="F52" s="1"/>
       <c r="G52" s="2"/>
       <c r="H52" s="30"/>
@@ -3501,9 +3459,9 @@
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
-      <c r="C53" s="91"/>
-      <c r="D53" s="92"/>
-      <c r="E53" s="93"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="34"/>
       <c r="F53" s="1"/>
       <c r="G53" s="2"/>
       <c r="H53" s="30"/>
@@ -3519,13 +3477,13 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="17"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="59"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="75"/>
       <c r="F54" s="18"/>
       <c r="G54" s="19"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="65"/>
+      <c r="H54" s="78"/>
+      <c r="I54" s="79"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
@@ -3536,90 +3494,104 @@
       <c r="Q54" s="21"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="95" t="s">
+      <c r="B55" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="96"/>
-      <c r="D55" s="96"/>
-      <c r="E55" s="96"/>
-      <c r="F55" s="97"/>
-      <c r="G55" s="98" t="s">
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="H55" s="99"/>
-      <c r="I55" s="99"/>
-      <c r="J55" s="99"/>
-      <c r="K55" s="100"/>
-      <c r="L55" s="100"/>
-      <c r="M55" s="100"/>
-      <c r="N55" s="102" t="s">
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="O55" s="100"/>
-      <c r="P55" s="100"/>
-      <c r="Q55" s="101"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="37"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="103"/>
-      <c r="C56" s="104"/>
-      <c r="D56" s="104"/>
-      <c r="E56" s="104"/>
-      <c r="F56" s="105"/>
-      <c r="G56" s="106"/>
-      <c r="H56" s="107"/>
-      <c r="I56" s="107"/>
-      <c r="J56" s="107"/>
-      <c r="K56" s="107"/>
-      <c r="L56" s="107"/>
-      <c r="M56" s="107"/>
-      <c r="N56" s="107"/>
-      <c r="O56" s="107"/>
-      <c r="P56" s="107"/>
-      <c r="Q56" s="108"/>
-      <c r="R56" s="109"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="40"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="41"/>
+      <c r="R56" s="42"/>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="110"/>
-      <c r="C57" s="111"/>
-      <c r="D57" s="111"/>
-      <c r="E57" s="111"/>
-      <c r="F57" s="112"/>
-      <c r="G57" s="113"/>
-      <c r="H57" s="114"/>
-      <c r="I57" s="114"/>
-      <c r="J57" s="114"/>
-      <c r="K57" s="114"/>
-      <c r="L57" s="114"/>
-      <c r="M57" s="114"/>
-      <c r="N57" s="114"/>
-      <c r="O57" s="114"/>
-      <c r="P57" s="114"/>
-      <c r="Q57" s="115"/>
-      <c r="R57" s="116"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="44"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="44"/>
+      <c r="O57" s="44"/>
+      <c r="P57" s="44"/>
+      <c r="Q57" s="45"/>
+      <c r="R57" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="B55:F57"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B1:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:Q16"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="H29:I29"/>
@@ -3634,42 +3606,28 @@
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C33:E33"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:Q16"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B55:F57"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
     <mergeCell ref="C54:E54"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B1:Q10"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
permirsimi i regjistrit perdhesa njesite
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
@@ -1137,6 +1137,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1170,51 +1308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1222,99 +1315,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1695,7 +1695,7 @@
   <dimension ref="B1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:I18"/>
+      <selection activeCell="H25" sqref="H25:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,244 +1718,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="58"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="89"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="91"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="61"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="89"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="61"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="89"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="90"/>
-      <c r="Q4" s="91"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="61"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="89"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="90"/>
-      <c r="N5" s="90"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="90"/>
-      <c r="Q5" s="91"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="61"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="91"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="61"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="89"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="91"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="61"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="89"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="91"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="61"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="89"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="91"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="61"/>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="93"/>
-      <c r="N10" s="93"/>
-      <c r="O10" s="93"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="94"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="64"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="96"/>
-      <c r="K11" s="96"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="96"/>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="97"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="67"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="99"/>
-      <c r="O12" s="99"/>
-      <c r="P12" s="99"/>
-      <c r="Q12" s="100"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="70"/>
     </row>
     <row r="13" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="101"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
-      <c r="N13" s="102"/>
-      <c r="O13" s="102"/>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="103"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="72"/>
+      <c r="P13" s="72"/>
+      <c r="Q13" s="73"/>
     </row>
     <row r="14" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -1970,18 +1970,18 @@
       <c r="E14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63" t="s">
+      <c r="G14" s="77"/>
+      <c r="H14" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="69" t="s">
+      <c r="I14" s="77"/>
+      <c r="J14" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="70"/>
+      <c r="K14" s="90"/>
       <c r="L14" s="8" t="s">
         <v>17</v>
       </c>
@@ -2014,18 +2014,18 @@
       <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="64">
+      <c r="F15" s="84">
         <v>411.35</v>
       </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="65" t="s">
+      <c r="G15" s="84"/>
+      <c r="H15" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="65"/>
-      <c r="J15" s="71" t="s">
+      <c r="I15" s="85"/>
+      <c r="J15" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="72"/>
+      <c r="K15" s="92"/>
       <c r="L15" s="11" t="s">
         <v>33</v>
       </c>
@@ -2046,62 +2046,62 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="68"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="88"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
-      <c r="M17" s="105"/>
-      <c r="N17" s="105"/>
-      <c r="O17" s="105"/>
-      <c r="P17" s="105"/>
-      <c r="Q17" s="106"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="76"/>
     </row>
     <row r="18" spans="2:17" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="83" t="s">
+      <c r="C18" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="85"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="28" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="76" t="s">
+      <c r="H18" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="77"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="28" t="s">
         <v>6</v>
       </c>
@@ -2131,21 +2131,21 @@
       <c r="B19" s="22">
         <v>1</v>
       </c>
-      <c r="C19" s="80" t="s">
+      <c r="C19" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="82"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="23">
         <v>3</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="80">
         <v>18.02</v>
       </c>
-      <c r="I19" s="59"/>
+      <c r="I19" s="81"/>
       <c r="J19" s="23" t="s">
         <v>34</v>
       </c>
@@ -2175,21 +2175,21 @@
       <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="80" t="s">
+      <c r="C20" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="82"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="23">
         <v>3</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="58">
+      <c r="H20" s="80">
         <v>14.64</v>
       </c>
-      <c r="I20" s="59"/>
+      <c r="I20" s="81"/>
       <c r="J20" s="23" t="s">
         <v>34</v>
       </c>
@@ -2219,21 +2219,21 @@
       <c r="B21" s="4">
         <v>3</v>
       </c>
-      <c r="C21" s="80" t="s">
+      <c r="C21" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="82"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="23">
         <v>4</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="58">
+      <c r="H21" s="80">
         <v>14.36</v>
       </c>
-      <c r="I21" s="59"/>
+      <c r="I21" s="81"/>
       <c r="J21" s="23" t="s">
         <v>34</v>
       </c>
@@ -2263,21 +2263,21 @@
       <c r="B22" s="4">
         <v>4</v>
       </c>
-      <c r="C22" s="80" t="s">
+      <c r="C22" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="81"/>
-      <c r="E22" s="82"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="52"/>
       <c r="F22" s="23">
         <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="58">
+      <c r="H22" s="80">
         <v>254.43</v>
       </c>
-      <c r="I22" s="59"/>
+      <c r="I22" s="81"/>
       <c r="J22" s="23" t="s">
         <v>34</v>
       </c>
@@ -2307,21 +2307,21 @@
       <c r="B23" s="22">
         <v>5</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="52"/>
       <c r="F23" s="23">
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="58">
-        <v>333.84</v>
-      </c>
-      <c r="I23" s="59"/>
+      <c r="H23" s="80">
+        <v>333.19</v>
+      </c>
+      <c r="I23" s="81"/>
       <c r="J23" s="23" t="s">
         <v>34</v>
       </c>
@@ -2351,21 +2351,21 @@
       <c r="B24" s="4">
         <v>6</v>
       </c>
-      <c r="C24" s="80" t="s">
+      <c r="C24" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="82"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
       <c r="F24" s="23">
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="58">
+      <c r="H24" s="80">
         <v>11.53</v>
       </c>
-      <c r="I24" s="59"/>
+      <c r="I24" s="81"/>
       <c r="J24" s="23" t="s">
         <v>34</v>
       </c>
@@ -2395,21 +2395,21 @@
       <c r="B25" s="22">
         <v>7</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="62"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="23">
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="58">
-        <v>12.41</v>
-      </c>
-      <c r="I25" s="59"/>
+      <c r="H25" s="80">
+        <v>12.71</v>
+      </c>
+      <c r="I25" s="81"/>
       <c r="J25" s="23" t="s">
         <v>34</v>
       </c>
@@ -2439,21 +2439,21 @@
       <c r="B26" s="4">
         <v>8</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
       </c>
-      <c r="H26" s="58">
+      <c r="H26" s="80">
         <v>333.67</v>
       </c>
-      <c r="I26" s="59"/>
+      <c r="I26" s="81"/>
       <c r="J26" s="23" t="s">
         <v>34</v>
       </c>
@@ -2483,21 +2483,21 @@
       <c r="B27" s="4">
         <v>9</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="62"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="1">
         <v>2</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
       </c>
-      <c r="H27" s="58">
+      <c r="H27" s="80">
         <v>12.28</v>
       </c>
-      <c r="I27" s="59"/>
+      <c r="I27" s="81"/>
       <c r="J27" s="23" t="s">
         <v>34</v>
       </c>
@@ -2527,21 +2527,21 @@
       <c r="B28" s="4">
         <v>10</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="H28" s="58">
+      <c r="H28" s="80">
         <v>11.82</v>
       </c>
-      <c r="I28" s="59"/>
+      <c r="I28" s="81"/>
       <c r="J28" s="23" t="s">
         <v>34</v>
       </c>
@@ -2571,21 +2571,21 @@
       <c r="B29" s="35">
         <v>11</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="62"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
       </c>
-      <c r="H29" s="58">
+      <c r="H29" s="80">
         <v>22.2</v>
       </c>
-      <c r="I29" s="59"/>
+      <c r="I29" s="81"/>
       <c r="J29" s="23" t="s">
         <v>34</v>
       </c>
@@ -2615,21 +2615,21 @@
       <c r="B30" s="35">
         <v>12</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="61"/>
-      <c r="E30" s="62"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="2">
         <v>2</v>
       </c>
-      <c r="H30" s="58">
+      <c r="H30" s="80">
         <v>20.6</v>
       </c>
-      <c r="I30" s="59"/>
+      <c r="I30" s="81"/>
       <c r="J30" s="23" t="s">
         <v>34</v>
       </c>
@@ -2659,21 +2659,21 @@
       <c r="B31" s="35">
         <v>13</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="62"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="2">
         <v>2</v>
       </c>
-      <c r="H31" s="58">
+      <c r="H31" s="80">
         <v>31.12</v>
       </c>
-      <c r="I31" s="59"/>
+      <c r="I31" s="81"/>
       <c r="J31" s="23" t="s">
         <v>34</v>
       </c>
@@ -2703,21 +2703,21 @@
       <c r="B32" s="35">
         <v>14</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="61"/>
-      <c r="E32" s="62"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="2">
         <v>2</v>
       </c>
-      <c r="H32" s="58">
+      <c r="H32" s="80">
         <v>32.97</v>
       </c>
-      <c r="I32" s="59"/>
+      <c r="I32" s="81"/>
       <c r="J32" s="23" t="s">
         <v>34</v>
       </c>
@@ -2747,21 +2747,21 @@
       <c r="B33" s="35">
         <v>15</v>
       </c>
-      <c r="C33" s="60" t="s">
+      <c r="C33" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="62"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="49"/>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="2">
         <v>2</v>
       </c>
-      <c r="H33" s="58">
+      <c r="H33" s="80">
         <v>30.53</v>
       </c>
-      <c r="I33" s="59">
+      <c r="I33" s="81">
         <v>30.53</v>
       </c>
       <c r="J33" s="23" t="s">
@@ -2793,21 +2793,21 @@
       <c r="B34" s="35">
         <v>16</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="C34" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="49"/>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="2">
         <v>2</v>
       </c>
-      <c r="H34" s="58">
+      <c r="H34" s="80">
         <v>26.02</v>
       </c>
-      <c r="I34" s="59">
+      <c r="I34" s="81">
         <v>26.02</v>
       </c>
       <c r="J34" s="23" t="s">
@@ -2839,21 +2839,21 @@
       <c r="B35" s="35">
         <v>17</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="62"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="49"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="2">
         <v>2</v>
       </c>
-      <c r="H35" s="58">
+      <c r="H35" s="80">
         <v>4.92</v>
       </c>
-      <c r="I35" s="59">
+      <c r="I35" s="81">
         <v>4.92</v>
       </c>
       <c r="J35" s="23" t="s">
@@ -2885,21 +2885,21 @@
       <c r="B36" s="35">
         <v>18</v>
       </c>
-      <c r="C36" s="60" t="s">
+      <c r="C36" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="61"/>
-      <c r="E36" s="62"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="49"/>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="2">
         <v>2</v>
       </c>
-      <c r="H36" s="58">
+      <c r="H36" s="80">
         <v>36.840000000000003</v>
       </c>
-      <c r="I36" s="59">
+      <c r="I36" s="81">
         <v>36.840000000000003</v>
       </c>
       <c r="J36" s="23" t="s">
@@ -2931,21 +2931,21 @@
       <c r="B37" s="35">
         <v>19</v>
       </c>
-      <c r="C37" s="60" t="s">
+      <c r="C37" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="62"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="2">
         <v>2</v>
       </c>
-      <c r="H37" s="58">
+      <c r="H37" s="80">
         <v>37.39</v>
       </c>
-      <c r="I37" s="59">
+      <c r="I37" s="81">
         <v>37.39</v>
       </c>
       <c r="J37" s="23" t="s">
@@ -2977,21 +2977,21 @@
       <c r="B38" s="35">
         <v>20</v>
       </c>
-      <c r="C38" s="60" t="s">
+      <c r="C38" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="61"/>
-      <c r="E38" s="62"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="H38" s="58">
+      <c r="H38" s="80">
         <v>35.07</v>
       </c>
-      <c r="I38" s="59">
+      <c r="I38" s="81">
         <v>35.07</v>
       </c>
       <c r="J38" s="23" t="s">
@@ -3023,21 +3023,21 @@
       <c r="B39" s="35">
         <v>21</v>
       </c>
-      <c r="C39" s="60" t="s">
+      <c r="C39" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="61"/>
-      <c r="E39" s="62"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="2">
         <v>2</v>
       </c>
-      <c r="H39" s="58">
+      <c r="H39" s="80">
         <v>37.89</v>
       </c>
-      <c r="I39" s="59">
+      <c r="I39" s="81">
         <v>37.89</v>
       </c>
       <c r="J39" s="23" t="s">
@@ -3069,11 +3069,11 @@
       <c r="B40" s="35">
         <v>22</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="61"/>
-      <c r="E40" s="62"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="49"/>
       <c r="F40" s="1">
         <v>1</v>
       </c>
@@ -3113,21 +3113,21 @@
       <c r="B41" s="35">
         <v>23</v>
       </c>
-      <c r="C41" s="60" t="s">
+      <c r="C41" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="61"/>
-      <c r="E41" s="62"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="49"/>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="2">
         <v>3</v>
       </c>
-      <c r="H41" s="58">
+      <c r="H41" s="80">
         <v>73.92</v>
       </c>
-      <c r="I41" s="59">
+      <c r="I41" s="81">
         <v>17.11</v>
       </c>
       <c r="J41" s="23" t="s">
@@ -3159,21 +3159,21 @@
       <c r="B42" s="35">
         <v>24</v>
       </c>
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="61"/>
-      <c r="E42" s="62"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="49"/>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="2">
         <v>3</v>
       </c>
-      <c r="H42" s="58">
+      <c r="H42" s="80">
         <v>32.96</v>
       </c>
-      <c r="I42" s="59"/>
+      <c r="I42" s="81"/>
       <c r="J42" s="23" t="s">
         <v>34</v>
       </c>
@@ -3203,21 +3203,21 @@
       <c r="B43" s="35">
         <v>25</v>
       </c>
-      <c r="C43" s="60" t="s">
+      <c r="C43" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49"/>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="2">
         <v>3</v>
       </c>
-      <c r="H43" s="58">
+      <c r="H43" s="80">
         <v>76.430000000000007</v>
       </c>
-      <c r="I43" s="59"/>
+      <c r="I43" s="81"/>
       <c r="J43" s="23" t="s">
         <v>34</v>
       </c>
@@ -3247,21 +3247,21 @@
       <c r="B44" s="35">
         <v>26</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="61"/>
-      <c r="E44" s="62"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="49"/>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="2">
         <v>3</v>
       </c>
-      <c r="H44" s="58">
+      <c r="H44" s="80">
         <v>86.27</v>
       </c>
-      <c r="I44" s="59"/>
+      <c r="I44" s="81"/>
       <c r="J44" s="23" t="s">
         <v>34</v>
       </c>
@@ -3291,21 +3291,21 @@
       <c r="B45" s="35">
         <v>27</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="62"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="49"/>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="2">
         <v>3</v>
       </c>
-      <c r="H45" s="58">
+      <c r="H45" s="80">
         <v>85.22</v>
       </c>
-      <c r="I45" s="59"/>
+      <c r="I45" s="81"/>
       <c r="J45" s="23" t="s">
         <v>34</v>
       </c>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="17"/>
-      <c r="C54" s="73"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="75"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="105"/>
+      <c r="E54" s="106"/>
       <c r="F54" s="18"/>
       <c r="G54" s="19"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="79"/>
+      <c r="H54" s="82"/>
+      <c r="I54" s="83"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
@@ -3494,19 +3494,19 @@
       <c r="Q54" s="21"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="56" t="s">
+      <c r="C55" s="94"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="95"/>
+      <c r="G55" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="H55" s="57"/>
-      <c r="I55" s="57"/>
-      <c r="J55" s="57"/>
+      <c r="H55" s="103"/>
+      <c r="I55" s="103"/>
+      <c r="J55" s="103"/>
       <c r="K55" s="36"/>
       <c r="L55" s="36"/>
       <c r="M55" s="36"/>
@@ -3518,11 +3518,11 @@
       <c r="Q55" s="37"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="50"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
-      <c r="E56" s="51"/>
-      <c r="F56" s="52"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="97"/>
+      <c r="D56" s="97"/>
+      <c r="E56" s="97"/>
+      <c r="F56" s="98"/>
       <c r="G56" s="39"/>
       <c r="H56" s="40"/>
       <c r="I56" s="40"/>
@@ -3537,11 +3537,11 @@
       <c r="R56" s="42"/>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="53"/>
-      <c r="C57" s="54"/>
-      <c r="D57" s="54"/>
-      <c r="E57" s="54"/>
-      <c r="F57" s="55"/>
+      <c r="B57" s="99"/>
+      <c r="C57" s="100"/>
+      <c r="D57" s="100"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="101"/>
       <c r="G57" s="43"/>
       <c r="H57" s="44"/>
       <c r="I57" s="44"/>
@@ -3557,41 +3557,23 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B1:Q10"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:Q16"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B55:F57"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="H29:I29"/>
@@ -3606,28 +3588,46 @@
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H20:I20"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B55:F57"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B1:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:Q16"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
permirsimi i regjistrit kati 1
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/16-Regjistri-për-ndërtesë-me-pjesë-të-ndërtesës-Dior.xlsx
@@ -1137,6 +1137,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1146,13 +1185,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1236,18 +1281,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1275,46 +1308,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1694,8 +1694,8 @@
   </sheetPr>
   <dimension ref="B1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:I25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,244 +1718,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="58"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="73"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="61"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="61"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="76"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="61"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="76"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="61"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="76"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="59"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="61"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="76"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="61"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="76"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="59"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="61"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="75"/>
+      <c r="O8" s="75"/>
+      <c r="P8" s="75"/>
+      <c r="Q8" s="76"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="61"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="76"/>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="62"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="64"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="79"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="67"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="82"/>
     </row>
     <row r="12" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="70"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="84"/>
+      <c r="L12" s="84"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="85"/>
     </row>
     <row r="13" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
-      <c r="M13" s="72"/>
-      <c r="N13" s="72"/>
-      <c r="O13" s="72"/>
-      <c r="P13" s="72"/>
-      <c r="Q13" s="73"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="88"/>
     </row>
     <row r="14" spans="2:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
@@ -1970,18 +1970,18 @@
       <c r="E14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77" t="s">
+      <c r="G14" s="92"/>
+      <c r="H14" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="77"/>
-      <c r="J14" s="89" t="s">
+      <c r="I14" s="92"/>
+      <c r="J14" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="90"/>
+      <c r="K14" s="101"/>
       <c r="L14" s="8" t="s">
         <v>17</v>
       </c>
@@ -2014,18 +2014,18 @@
       <c r="E15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="84">
+      <c r="F15" s="95">
         <v>411.35</v>
       </c>
-      <c r="G15" s="84"/>
-      <c r="H15" s="85" t="s">
+      <c r="G15" s="95"/>
+      <c r="H15" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="85"/>
-      <c r="J15" s="91" t="s">
+      <c r="I15" s="96"/>
+      <c r="J15" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="92"/>
+      <c r="K15" s="103"/>
       <c r="L15" s="11" t="s">
         <v>33</v>
       </c>
@@ -2046,62 +2046,62 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="86"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="88"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="98"/>
+      <c r="L16" s="98"/>
+      <c r="M16" s="98"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="98"/>
+      <c r="P16" s="98"/>
+      <c r="Q16" s="99"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="76"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="91"/>
     </row>
     <row r="18" spans="2:17" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="54"/>
-      <c r="E18" s="55"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="70"/>
       <c r="F18" s="28" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="H18" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="79"/>
+      <c r="I18" s="94"/>
       <c r="J18" s="28" t="s">
         <v>6</v>
       </c>
@@ -2131,21 +2131,21 @@
       <c r="B19" s="22">
         <v>1</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="106"/>
       <c r="F19" s="23">
         <v>3</v>
       </c>
       <c r="G19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="80">
+      <c r="H19" s="58">
         <v>18.02</v>
       </c>
-      <c r="I19" s="81"/>
+      <c r="I19" s="59"/>
       <c r="J19" s="23" t="s">
         <v>34</v>
       </c>
@@ -2175,21 +2175,21 @@
       <c r="B20" s="4">
         <v>2</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="106"/>
       <c r="F20" s="23">
         <v>3</v>
       </c>
       <c r="G20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="80">
+      <c r="H20" s="58">
         <v>14.64</v>
       </c>
-      <c r="I20" s="81"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="23" t="s">
         <v>34</v>
       </c>
@@ -2219,21 +2219,21 @@
       <c r="B21" s="4">
         <v>3</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="106"/>
       <c r="F21" s="23">
         <v>4</v>
       </c>
       <c r="G21" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="80">
+      <c r="H21" s="58">
         <v>14.36</v>
       </c>
-      <c r="I21" s="81"/>
+      <c r="I21" s="59"/>
       <c r="J21" s="23" t="s">
         <v>34</v>
       </c>
@@ -2263,21 +2263,21 @@
       <c r="B22" s="4">
         <v>4</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="106"/>
       <c r="F22" s="23">
         <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="80">
+      <c r="H22" s="58">
         <v>254.43</v>
       </c>
-      <c r="I22" s="81"/>
+      <c r="I22" s="59"/>
       <c r="J22" s="23" t="s">
         <v>34</v>
       </c>
@@ -2307,21 +2307,21 @@
       <c r="B23" s="22">
         <v>5</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="106"/>
       <c r="F23" s="23">
         <v>2</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="80">
+      <c r="H23" s="58">
         <v>333.19</v>
       </c>
-      <c r="I23" s="81"/>
+      <c r="I23" s="59"/>
       <c r="J23" s="23" t="s">
         <v>34</v>
       </c>
@@ -2351,21 +2351,21 @@
       <c r="B24" s="4">
         <v>6</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="52"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="106"/>
       <c r="F24" s="23">
         <v>2</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="80">
+      <c r="H24" s="58">
         <v>11.53</v>
       </c>
-      <c r="I24" s="81"/>
+      <c r="I24" s="59"/>
       <c r="J24" s="23" t="s">
         <v>34</v>
       </c>
@@ -2395,21 +2395,21 @@
       <c r="B25" s="22">
         <v>7</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="49"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="23">
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="80">
+      <c r="H25" s="58">
         <v>12.71</v>
       </c>
-      <c r="I25" s="81"/>
+      <c r="I25" s="59"/>
       <c r="J25" s="23" t="s">
         <v>34</v>
       </c>
@@ -2439,21 +2439,21 @@
       <c r="B26" s="4">
         <v>8</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="2">
         <v>1</v>
       </c>
-      <c r="H26" s="80">
-        <v>333.67</v>
-      </c>
-      <c r="I26" s="81"/>
+      <c r="H26" s="58">
+        <v>333.34</v>
+      </c>
+      <c r="I26" s="59"/>
       <c r="J26" s="23" t="s">
         <v>34</v>
       </c>
@@ -2483,21 +2483,21 @@
       <c r="B27" s="4">
         <v>9</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="49"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="1">
         <v>2</v>
       </c>
       <c r="G27" s="2">
         <v>1</v>
       </c>
-      <c r="H27" s="80">
-        <v>12.28</v>
-      </c>
-      <c r="I27" s="81"/>
+      <c r="H27" s="58">
+        <v>11.38</v>
+      </c>
+      <c r="I27" s="59"/>
       <c r="J27" s="23" t="s">
         <v>34</v>
       </c>
@@ -2527,21 +2527,21 @@
       <c r="B28" s="4">
         <v>10</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="62"/>
       <c r="F28" s="1">
         <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>1</v>
       </c>
-      <c r="H28" s="80">
-        <v>11.82</v>
-      </c>
-      <c r="I28" s="81"/>
+      <c r="H28" s="58">
+        <v>10.58</v>
+      </c>
+      <c r="I28" s="59"/>
       <c r="J28" s="23" t="s">
         <v>34</v>
       </c>
@@ -2571,21 +2571,21 @@
       <c r="B29" s="35">
         <v>11</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="48"/>
-      <c r="E29" s="49"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
       </c>
-      <c r="H29" s="80">
+      <c r="H29" s="58">
         <v>22.2</v>
       </c>
-      <c r="I29" s="81"/>
+      <c r="I29" s="59"/>
       <c r="J29" s="23" t="s">
         <v>34</v>
       </c>
@@ -2615,21 +2615,21 @@
       <c r="B30" s="35">
         <v>12</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="62"/>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="2">
         <v>2</v>
       </c>
-      <c r="H30" s="80">
+      <c r="H30" s="58">
         <v>20.6</v>
       </c>
-      <c r="I30" s="81"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="23" t="s">
         <v>34</v>
       </c>
@@ -2659,21 +2659,21 @@
       <c r="B31" s="35">
         <v>13</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="48"/>
-      <c r="E31" s="49"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="62"/>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="2">
         <v>2</v>
       </c>
-      <c r="H31" s="80">
+      <c r="H31" s="58">
         <v>31.12</v>
       </c>
-      <c r="I31" s="81"/>
+      <c r="I31" s="59"/>
       <c r="J31" s="23" t="s">
         <v>34</v>
       </c>
@@ -2703,21 +2703,21 @@
       <c r="B32" s="35">
         <v>14</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="62"/>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="2">
         <v>2</v>
       </c>
-      <c r="H32" s="80">
+      <c r="H32" s="58">
         <v>32.97</v>
       </c>
-      <c r="I32" s="81"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="23" t="s">
         <v>34</v>
       </c>
@@ -2747,21 +2747,21 @@
       <c r="B33" s="35">
         <v>15</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="49"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="62"/>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="2">
         <v>2</v>
       </c>
-      <c r="H33" s="80">
+      <c r="H33" s="58">
         <v>30.53</v>
       </c>
-      <c r="I33" s="81">
+      <c r="I33" s="59">
         <v>30.53</v>
       </c>
       <c r="J33" s="23" t="s">
@@ -2793,21 +2793,21 @@
       <c r="B34" s="35">
         <v>16</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="49"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="62"/>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="2">
         <v>2</v>
       </c>
-      <c r="H34" s="80">
+      <c r="H34" s="58">
         <v>26.02</v>
       </c>
-      <c r="I34" s="81">
+      <c r="I34" s="59">
         <v>26.02</v>
       </c>
       <c r="J34" s="23" t="s">
@@ -2839,21 +2839,21 @@
       <c r="B35" s="35">
         <v>17</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="49"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="62"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="2">
         <v>2</v>
       </c>
-      <c r="H35" s="80">
+      <c r="H35" s="58">
         <v>4.92</v>
       </c>
-      <c r="I35" s="81">
+      <c r="I35" s="59">
         <v>4.92</v>
       </c>
       <c r="J35" s="23" t="s">
@@ -2885,21 +2885,21 @@
       <c r="B36" s="35">
         <v>18</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="62"/>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="2">
         <v>2</v>
       </c>
-      <c r="H36" s="80">
+      <c r="H36" s="58">
         <v>36.840000000000003</v>
       </c>
-      <c r="I36" s="81">
+      <c r="I36" s="59">
         <v>36.840000000000003</v>
       </c>
       <c r="J36" s="23" t="s">
@@ -2931,21 +2931,21 @@
       <c r="B37" s="35">
         <v>19</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="62"/>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="2">
         <v>2</v>
       </c>
-      <c r="H37" s="80">
+      <c r="H37" s="58">
         <v>37.39</v>
       </c>
-      <c r="I37" s="81">
+      <c r="I37" s="59">
         <v>37.39</v>
       </c>
       <c r="J37" s="23" t="s">
@@ -2977,21 +2977,21 @@
       <c r="B38" s="35">
         <v>20</v>
       </c>
-      <c r="C38" s="47" t="s">
+      <c r="C38" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="48"/>
-      <c r="E38" s="49"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="2">
         <v>2</v>
       </c>
-      <c r="H38" s="80">
+      <c r="H38" s="58">
         <v>35.07</v>
       </c>
-      <c r="I38" s="81">
+      <c r="I38" s="59">
         <v>35.07</v>
       </c>
       <c r="J38" s="23" t="s">
@@ -3023,21 +3023,21 @@
       <c r="B39" s="35">
         <v>21</v>
       </c>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="49"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="62"/>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="2">
         <v>2</v>
       </c>
-      <c r="H39" s="80">
+      <c r="H39" s="58">
         <v>37.89</v>
       </c>
-      <c r="I39" s="81">
+      <c r="I39" s="59">
         <v>37.89</v>
       </c>
       <c r="J39" s="23" t="s">
@@ -3069,11 +3069,11 @@
       <c r="B40" s="35">
         <v>22</v>
       </c>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="49"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="62"/>
       <c r="F40" s="1">
         <v>1</v>
       </c>
@@ -3113,21 +3113,21 @@
       <c r="B41" s="35">
         <v>23</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="49"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="62"/>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="2">
         <v>3</v>
       </c>
-      <c r="H41" s="80">
+      <c r="H41" s="58">
         <v>73.92</v>
       </c>
-      <c r="I41" s="81">
+      <c r="I41" s="59">
         <v>17.11</v>
       </c>
       <c r="J41" s="23" t="s">
@@ -3159,21 +3159,21 @@
       <c r="B42" s="35">
         <v>24</v>
       </c>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="62"/>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="2">
         <v>3</v>
       </c>
-      <c r="H42" s="80">
+      <c r="H42" s="58">
         <v>32.96</v>
       </c>
-      <c r="I42" s="81"/>
+      <c r="I42" s="59"/>
       <c r="J42" s="23" t="s">
         <v>34</v>
       </c>
@@ -3203,21 +3203,21 @@
       <c r="B43" s="35">
         <v>25</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="49"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62"/>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="2">
         <v>3</v>
       </c>
-      <c r="H43" s="80">
+      <c r="H43" s="58">
         <v>76.430000000000007</v>
       </c>
-      <c r="I43" s="81"/>
+      <c r="I43" s="59"/>
       <c r="J43" s="23" t="s">
         <v>34</v>
       </c>
@@ -3247,21 +3247,21 @@
       <c r="B44" s="35">
         <v>26</v>
       </c>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="2">
         <v>3</v>
       </c>
-      <c r="H44" s="80">
+      <c r="H44" s="58">
         <v>86.27</v>
       </c>
-      <c r="I44" s="81"/>
+      <c r="I44" s="59"/>
       <c r="J44" s="23" t="s">
         <v>34</v>
       </c>
@@ -3291,21 +3291,21 @@
       <c r="B45" s="35">
         <v>27</v>
       </c>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="48"/>
-      <c r="E45" s="49"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="62"/>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="2">
         <v>3</v>
       </c>
-      <c r="H45" s="80">
+      <c r="H45" s="58">
         <v>85.22</v>
       </c>
-      <c r="I45" s="81"/>
+      <c r="I45" s="59"/>
       <c r="J45" s="23" t="s">
         <v>34</v>
       </c>
@@ -3477,13 +3477,13 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="17"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="105"/>
-      <c r="E54" s="106"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="65"/>
       <c r="F54" s="18"/>
       <c r="G54" s="19"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="83"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="67"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
@@ -3494,19 +3494,19 @@
       <c r="Q54" s="21"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="93" t="s">
+      <c r="B55" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="94"/>
-      <c r="D55" s="94"/>
-      <c r="E55" s="94"/>
-      <c r="F55" s="95"/>
-      <c r="G55" s="102" t="s">
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="H55" s="103"/>
-      <c r="I55" s="103"/>
-      <c r="J55" s="103"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
       <c r="K55" s="36"/>
       <c r="L55" s="36"/>
       <c r="M55" s="36"/>
@@ -3518,11 +3518,11 @@
       <c r="Q55" s="37"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="96"/>
-      <c r="C56" s="97"/>
-      <c r="D56" s="97"/>
-      <c r="E56" s="97"/>
-      <c r="F56" s="98"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="52"/>
       <c r="G56" s="39"/>
       <c r="H56" s="40"/>
       <c r="I56" s="40"/>
@@ -3537,11 +3537,11 @@
       <c r="R56" s="42"/>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="99"/>
-      <c r="C57" s="100"/>
-      <c r="D57" s="100"/>
-      <c r="E57" s="100"/>
-      <c r="F57" s="101"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55"/>
       <c r="G57" s="43"/>
       <c r="H57" s="44"/>
       <c r="I57" s="44"/>
@@ -3557,37 +3557,30 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="B55:F57"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B1:Q10"/>
+    <mergeCell ref="B11:Q11"/>
+    <mergeCell ref="B12:Q12"/>
+    <mergeCell ref="B13:Q13"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B16:Q16"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="H54:I54"/>
     <mergeCell ref="H28:I28"/>
@@ -3604,30 +3597,37 @@
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="H39:I39"/>
     <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B1:Q10"/>
-    <mergeCell ref="B11:Q11"/>
-    <mergeCell ref="B12:Q12"/>
-    <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B16:Q16"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B55:F57"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C54:E54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>